<commit_message>
Ajout du camembert GICS sectoriel dans la page Positions Mensuelles
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/soltanirayen/Desktop/virtual_ptf/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/soltanirayen/Desktop/SBR_Portfolio_App/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5367792-6BEA-F644-8494-B37B05DC96E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00D2CBCA-CF71-8749-9436-347D5DE42911}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ordres" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="895" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1295" uniqueCount="265">
   <si>
     <t>Date</t>
   </si>
@@ -567,6 +567,273 @@
   <si>
     <t>Performance</t>
   </si>
+  <si>
+    <t>US00206R1023</t>
+  </si>
+  <si>
+    <t>Communication Services</t>
+  </si>
+  <si>
+    <t>US05464C1018</t>
+  </si>
+  <si>
+    <t>Industrials</t>
+  </si>
+  <si>
+    <t>US1011371077</t>
+  </si>
+  <si>
+    <t>Health Care</t>
+  </si>
+  <si>
+    <t>US11135F1012</t>
+  </si>
+  <si>
+    <t>Information Technology</t>
+  </si>
+  <si>
+    <t>US21037T1097</t>
+  </si>
+  <si>
+    <t>Utilities</t>
+  </si>
+  <si>
+    <t>US22052L1044</t>
+  </si>
+  <si>
+    <t>Materials</t>
+  </si>
+  <si>
+    <t>US23918K1088</t>
+  </si>
+  <si>
+    <t>US2786421030</t>
+  </si>
+  <si>
+    <t>Consumer Discretionary</t>
+  </si>
+  <si>
+    <t>US5324571083</t>
+  </si>
+  <si>
+    <t>US3696043013</t>
+  </si>
+  <si>
+    <t>US4432011082</t>
+  </si>
+  <si>
+    <t>US4601461035</t>
+  </si>
+  <si>
+    <t>IE00BY7QL619</t>
+  </si>
+  <si>
+    <t>US4878361082</t>
+  </si>
+  <si>
+    <t>Consumer Staples</t>
+  </si>
+  <si>
+    <t>US30303M1027</t>
+  </si>
+  <si>
+    <t>US64110L1061</t>
+  </si>
+  <si>
+    <t>US6293775085</t>
+  </si>
+  <si>
+    <t>US67066G1040</t>
+  </si>
+  <si>
+    <t>US6826801036</t>
+  </si>
+  <si>
+    <t>Energy</t>
+  </si>
+  <si>
+    <t>US6951561090</t>
+  </si>
+  <si>
+    <t>US69608A1088</t>
+  </si>
+  <si>
+    <t>US7445731067</t>
+  </si>
+  <si>
+    <t>US7512121010</t>
+  </si>
+  <si>
+    <t>US87612G1013</t>
+  </si>
+  <si>
+    <t>US88262P1021</t>
+  </si>
+  <si>
+    <t>US5010441013</t>
+  </si>
+  <si>
+    <t>US9694571004</t>
+  </si>
+  <si>
+    <t>US92840M1027</t>
+  </si>
+  <si>
+    <t>US9311421039</t>
+  </si>
+  <si>
+    <t>US9699041011</t>
+  </si>
+  <si>
+    <t>US88579Y1010</t>
+  </si>
+  <si>
+    <t>US0091581068</t>
+  </si>
+  <si>
+    <t>US02209S1033</t>
+  </si>
+  <si>
+    <t>US09857L1089</t>
+  </si>
+  <si>
+    <t>US29364G1031</t>
+  </si>
+  <si>
+    <t>US35137L1052</t>
+  </si>
+  <si>
+    <t>CH0114405324</t>
+  </si>
+  <si>
+    <t>US36828A1016</t>
+  </si>
+  <si>
+    <t>US3802371076</t>
+  </si>
+  <si>
+    <t>US45784P1012</t>
+  </si>
+  <si>
+    <t>US46120E6023</t>
+  </si>
+  <si>
+    <t>US49456B1017</t>
+  </si>
+  <si>
+    <t>US6516391066</t>
+  </si>
+  <si>
+    <t>US65473P1057</t>
+  </si>
+  <si>
+    <t>US7181721090</t>
+  </si>
+  <si>
+    <t>LR0008862868</t>
+  </si>
+  <si>
+    <t>US8725901040</t>
+  </si>
+  <si>
+    <t>US0236081024</t>
+  </si>
+  <si>
+    <t>US3156161024</t>
+  </si>
+  <si>
+    <t>US3032501047</t>
+  </si>
+  <si>
+    <t>US3755581036</t>
+  </si>
+  <si>
+    <t>US8760301072</t>
+  </si>
+  <si>
+    <t>US25809K1051</t>
+  </si>
+  <si>
+    <t>US34959E1091</t>
+  </si>
+  <si>
+    <t>US5380341090</t>
+  </si>
+  <si>
+    <t>US8740541094</t>
+  </si>
+  <si>
+    <t>US9100471096</t>
+  </si>
+  <si>
+    <t>US92939U1060</t>
+  </si>
+  <si>
+    <t>US1101221083</t>
+  </si>
+  <si>
+    <t>PA1436583006</t>
+  </si>
+  <si>
+    <t>US12504L1098</t>
+  </si>
+  <si>
+    <t>Real Estate</t>
+  </si>
+  <si>
+    <t>US2473617023</t>
+  </si>
+  <si>
+    <t>US46284V1017</t>
+  </si>
+  <si>
+    <t>BMG667211046</t>
+  </si>
+  <si>
+    <t>US70432V1026</t>
+  </si>
+  <si>
+    <t>US88160R1014</t>
+  </si>
+  <si>
+    <t>US02079K3059</t>
+  </si>
+  <si>
+    <t>US0231351067</t>
+  </si>
+  <si>
+    <t>US0378331005</t>
+  </si>
+  <si>
+    <t>IE00B4BNMY34</t>
+  </si>
+  <si>
+    <t>US00724F1012</t>
+  </si>
+  <si>
+    <t>US31428X1063</t>
+  </si>
+  <si>
+    <t>US6541061031</t>
+  </si>
+  <si>
+    <t>US15189T1079</t>
+  </si>
+  <si>
+    <t>US2371941053</t>
+  </si>
+  <si>
+    <t>US2566771059</t>
+  </si>
+  <si>
+    <t>US2333311072</t>
+  </si>
+  <si>
+    <t>US30161N1019</t>
+  </si>
+  <si>
+    <t>US92343E1029</t>
+  </si>
 </sst>
 </file>
 
@@ -725,7 +992,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -818,9 +1085,6 @@
     <xf numFmtId="10" fontId="2" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1129,7 +1393,9 @@
   </sheetPr>
   <dimension ref="A1:K201"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1137,8 +1403,8 @@
     <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="56" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="45.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10" style="23" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.33203125" style="7" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="6.83203125" bestFit="1" customWidth="1"/>
@@ -1194,8 +1460,12 @@
       <c r="D2" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
+      <c r="E2" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>177</v>
+      </c>
       <c r="G2" s="13">
         <v>110</v>
       </c>
@@ -1226,8 +1496,12 @@
       <c r="D3" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
+      <c r="E3" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>179</v>
+      </c>
       <c r="G3" s="18">
         <v>12</v>
       </c>
@@ -1258,8 +1532,12 @@
       <c r="D4" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
+      <c r="E4" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>181</v>
+      </c>
       <c r="G4" s="13">
         <v>52</v>
       </c>
@@ -1290,8 +1568,12 @@
       <c r="D5" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
+      <c r="E5" s="17" t="s">
+        <v>182</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>183</v>
+      </c>
       <c r="G5" s="18">
         <v>10</v>
       </c>
@@ -1322,8 +1604,12 @@
       <c r="D6" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
+      <c r="E6" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>185</v>
+      </c>
       <c r="G6" s="13">
         <v>28</v>
       </c>
@@ -1354,8 +1640,12 @@
       <c r="D7" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
+      <c r="E7" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="F7" s="17" t="s">
+        <v>187</v>
+      </c>
       <c r="G7" s="18">
         <v>69</v>
       </c>
@@ -1386,8 +1676,12 @@
       <c r="D8" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
+      <c r="E8" s="12" t="s">
+        <v>188</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>181</v>
+      </c>
       <c r="G8" s="13">
         <v>10</v>
       </c>
@@ -1418,8 +1712,12 @@
       <c r="D9" s="17" t="s">
         <v>99</v>
       </c>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
+      <c r="E9" s="17" t="s">
+        <v>189</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>190</v>
+      </c>
       <c r="G9" s="18">
         <v>77</v>
       </c>
@@ -1450,8 +1748,12 @@
       <c r="D10" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
+      <c r="E10" s="12" t="s">
+        <v>191</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>181</v>
+      </c>
       <c r="G10" s="13">
         <v>4</v>
       </c>
@@ -1482,8 +1784,12 @@
       <c r="D11" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
+      <c r="E11" s="17" t="s">
+        <v>192</v>
+      </c>
+      <c r="F11" s="17" t="s">
+        <v>179</v>
+      </c>
       <c r="G11" s="18">
         <v>31</v>
       </c>
@@ -1514,8 +1820,12 @@
       <c r="D12" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
+      <c r="E12" s="12" t="s">
+        <v>193</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>179</v>
+      </c>
       <c r="G12" s="13">
         <v>59</v>
       </c>
@@ -1546,8 +1856,12 @@
       <c r="D13" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
+      <c r="E13" s="17" t="s">
+        <v>194</v>
+      </c>
+      <c r="F13" s="17" t="s">
+        <v>187</v>
+      </c>
       <c r="G13" s="18">
         <v>84</v>
       </c>
@@ -1578,8 +1892,12 @@
       <c r="D14" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
+      <c r="E14" s="12" t="s">
+        <v>195</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>179</v>
+      </c>
       <c r="G14" s="13">
         <v>60</v>
       </c>
@@ -1610,8 +1928,12 @@
       <c r="D15" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
+      <c r="E15" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="F15" s="17" t="s">
+        <v>197</v>
+      </c>
       <c r="G15" s="18">
         <v>58</v>
       </c>
@@ -1642,8 +1964,12 @@
       <c r="D16" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
+      <c r="E16" s="12" t="s">
+        <v>198</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>177</v>
+      </c>
       <c r="G16" s="13">
         <v>8</v>
       </c>
@@ -1674,8 +2000,12 @@
       <c r="D17" s="17" t="s">
         <v>107</v>
       </c>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
+      <c r="E17" s="17" t="s">
+        <v>199</v>
+      </c>
+      <c r="F17" s="17" t="s">
+        <v>177</v>
+      </c>
       <c r="G17" s="18">
         <v>4</v>
       </c>
@@ -1706,8 +2036,12 @@
       <c r="D18" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
+      <c r="E18" s="12" t="s">
+        <v>200</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>185</v>
+      </c>
       <c r="G18" s="13">
         <v>62</v>
       </c>
@@ -1738,8 +2072,12 @@
       <c r="D19" s="17" t="s">
         <v>109</v>
       </c>
-      <c r="E19" s="17"/>
-      <c r="F19" s="17"/>
+      <c r="E19" s="17" t="s">
+        <v>201</v>
+      </c>
+      <c r="F19" s="17" t="s">
+        <v>183</v>
+      </c>
       <c r="G19" s="18">
         <v>56</v>
       </c>
@@ -1770,8 +2108,12 @@
       <c r="D20" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
+      <c r="E20" s="12" t="s">
+        <v>202</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>203</v>
+      </c>
       <c r="G20" s="13">
         <v>45</v>
       </c>
@@ -1802,8 +2144,12 @@
       <c r="D21" s="17" t="s">
         <v>111</v>
       </c>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
+      <c r="E21" s="17" t="s">
+        <v>204</v>
+      </c>
+      <c r="F21" s="17" t="s">
+        <v>187</v>
+      </c>
       <c r="G21" s="18">
         <v>19</v>
       </c>
@@ -1834,8 +2180,12 @@
       <c r="D22" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
+      <c r="E22" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="F22" s="12" t="s">
+        <v>183</v>
+      </c>
       <c r="G22" s="13">
         <v>110</v>
       </c>
@@ -1866,8 +2216,12 @@
       <c r="D23" s="17" t="s">
         <v>113</v>
       </c>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17"/>
+      <c r="E23" s="17" t="s">
+        <v>206</v>
+      </c>
+      <c r="F23" s="17" t="s">
+        <v>185</v>
+      </c>
       <c r="G23" s="18">
         <v>53</v>
       </c>
@@ -1898,8 +2252,12 @@
       <c r="D24" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
+      <c r="E24" s="12" t="s">
+        <v>207</v>
+      </c>
+      <c r="F24" s="12" t="s">
+        <v>190</v>
+      </c>
       <c r="G24" s="13">
         <v>23</v>
       </c>
@@ -1930,8 +2288,12 @@
       <c r="D25" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="E25" s="17"/>
-      <c r="F25" s="17"/>
+      <c r="E25" s="17" t="s">
+        <v>208</v>
+      </c>
+      <c r="F25" s="17" t="s">
+        <v>203</v>
+      </c>
       <c r="G25" s="18">
         <v>38</v>
       </c>
@@ -1962,8 +2324,12 @@
       <c r="D26" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
+      <c r="E26" s="12" t="s">
+        <v>209</v>
+      </c>
+      <c r="F26" s="12" t="s">
+        <v>203</v>
+      </c>
       <c r="G26" s="13">
         <v>6</v>
       </c>
@@ -1994,8 +2360,12 @@
       <c r="D27" s="17" t="s">
         <v>117</v>
       </c>
-      <c r="E27" s="17"/>
-      <c r="F27" s="17"/>
+      <c r="E27" s="17" t="s">
+        <v>210</v>
+      </c>
+      <c r="F27" s="17" t="s">
+        <v>197</v>
+      </c>
       <c r="G27" s="18">
         <v>68</v>
       </c>
@@ -2026,8 +2396,12 @@
       <c r="D28" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="E28" s="12"/>
-      <c r="F28" s="12"/>
+      <c r="E28" s="12" t="s">
+        <v>211</v>
+      </c>
+      <c r="F28" s="12" t="s">
+        <v>203</v>
+      </c>
       <c r="G28" s="13">
         <v>91</v>
       </c>
@@ -2058,8 +2432,12 @@
       <c r="D29" s="17" t="s">
         <v>119</v>
       </c>
-      <c r="E29" s="17"/>
-      <c r="F29" s="17"/>
+      <c r="E29" s="17" t="s">
+        <v>212</v>
+      </c>
+      <c r="F29" s="17" t="s">
+        <v>185</v>
+      </c>
       <c r="G29" s="18">
         <v>80</v>
       </c>
@@ -2090,8 +2468,12 @@
       <c r="D30" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="E30" s="12"/>
-      <c r="F30" s="12"/>
+      <c r="E30" s="12" t="s">
+        <v>213</v>
+      </c>
+      <c r="F30" s="12" t="s">
+        <v>197</v>
+      </c>
       <c r="G30" s="13">
         <v>58</v>
       </c>
@@ -2122,8 +2504,12 @@
       <c r="D31" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="E31" s="17"/>
-      <c r="F31" s="17"/>
+      <c r="E31" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="F31" s="17" t="s">
+        <v>190</v>
+      </c>
       <c r="G31" s="18">
         <v>31</v>
       </c>
@@ -2154,8 +2540,12 @@
       <c r="D32" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="E32" s="12"/>
-      <c r="F32" s="12"/>
+      <c r="E32" s="12" t="s">
+        <v>215</v>
+      </c>
+      <c r="F32" s="12" t="s">
+        <v>179</v>
+      </c>
       <c r="G32" s="13">
         <v>33</v>
       </c>
@@ -2186,8 +2576,12 @@
       <c r="D33" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="E33" s="17"/>
-      <c r="F33" s="17"/>
+      <c r="E33" s="17" t="s">
+        <v>216</v>
+      </c>
+      <c r="F33" s="17" t="s">
+        <v>187</v>
+      </c>
       <c r="G33" s="18">
         <v>13</v>
       </c>
@@ -2218,8 +2612,12 @@
       <c r="D34" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="E34" s="12"/>
-      <c r="F34" s="12"/>
+      <c r="E34" s="12" t="s">
+        <v>217</v>
+      </c>
+      <c r="F34" s="12" t="s">
+        <v>197</v>
+      </c>
       <c r="G34" s="13">
         <v>73</v>
       </c>
@@ -2250,8 +2648,12 @@
       <c r="D35" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="E35" s="17"/>
-      <c r="F35" s="17"/>
+      <c r="E35" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="F35" s="17" t="s">
+        <v>179</v>
+      </c>
       <c r="G35" s="18">
         <v>12</v>
       </c>
@@ -2282,8 +2684,12 @@
       <c r="D36" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="E36" s="12"/>
-      <c r="F36" s="12"/>
+      <c r="E36" s="12" t="s">
+        <v>218</v>
+      </c>
+      <c r="F36" s="12" t="s">
+        <v>190</v>
+      </c>
       <c r="G36" s="13">
         <v>1</v>
       </c>
@@ -2314,8 +2720,12 @@
       <c r="D37" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="E37" s="17"/>
-      <c r="F37" s="17"/>
+      <c r="E37" s="17" t="s">
+        <v>184</v>
+      </c>
+      <c r="F37" s="17" t="s">
+        <v>185</v>
+      </c>
       <c r="G37" s="18">
         <v>28</v>
       </c>
@@ -2346,8 +2756,12 @@
       <c r="D38" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="E38" s="12"/>
-      <c r="F38" s="12"/>
+      <c r="E38" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="F38" s="12" t="s">
+        <v>187</v>
+      </c>
       <c r="G38" s="13">
         <v>69</v>
       </c>
@@ -2378,8 +2792,12 @@
       <c r="D39" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="E39" s="17"/>
-      <c r="F39" s="17"/>
+      <c r="E39" s="17" t="s">
+        <v>188</v>
+      </c>
+      <c r="F39" s="17" t="s">
+        <v>181</v>
+      </c>
       <c r="G39" s="18">
         <v>10</v>
       </c>
@@ -2410,8 +2828,12 @@
       <c r="D40" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="E40" s="12"/>
-      <c r="F40" s="12"/>
+      <c r="E40" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="F40" s="12" t="s">
+        <v>190</v>
+      </c>
       <c r="G40" s="13">
         <v>77</v>
       </c>
@@ -2442,8 +2864,12 @@
       <c r="D41" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="E41" s="17"/>
-      <c r="F41" s="17"/>
+      <c r="E41" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="F41" s="17" t="s">
+        <v>181</v>
+      </c>
       <c r="G41" s="18">
         <v>4</v>
       </c>
@@ -2474,8 +2900,12 @@
       <c r="D42" s="12" t="s">
         <v>127</v>
       </c>
-      <c r="E42" s="12"/>
-      <c r="F42" s="12"/>
+      <c r="E42" s="12" t="s">
+        <v>219</v>
+      </c>
+      <c r="F42" s="12" t="s">
+        <v>185</v>
+      </c>
       <c r="G42" s="13">
         <v>60</v>
       </c>
@@ -2506,8 +2936,12 @@
       <c r="D43" s="17" t="s">
         <v>128</v>
       </c>
-      <c r="E43" s="17"/>
-      <c r="F43" s="17"/>
+      <c r="E43" s="17" t="s">
+        <v>220</v>
+      </c>
+      <c r="F43" s="17" t="s">
+        <v>177</v>
+      </c>
       <c r="G43" s="18">
         <v>101</v>
       </c>
@@ -2538,8 +2972,12 @@
       <c r="D44" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="E44" s="12"/>
-      <c r="F44" s="12"/>
+      <c r="E44" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="F44" s="12" t="s">
+        <v>190</v>
+      </c>
       <c r="G44" s="13">
         <v>21</v>
       </c>
@@ -2570,8 +3008,12 @@
       <c r="D45" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="E45" s="17"/>
-      <c r="F45" s="17"/>
+      <c r="E45" s="17" t="s">
+        <v>222</v>
+      </c>
+      <c r="F45" s="17" t="s">
+        <v>179</v>
+      </c>
       <c r="G45" s="18">
         <v>22</v>
       </c>
@@ -2602,8 +3044,12 @@
       <c r="D46" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="E46" s="12"/>
-      <c r="F46" s="12"/>
+      <c r="E46" s="12" t="s">
+        <v>192</v>
+      </c>
+      <c r="F46" s="12" t="s">
+        <v>179</v>
+      </c>
       <c r="G46" s="13">
         <v>31</v>
       </c>
@@ -2634,8 +3080,12 @@
       <c r="D47" s="17" t="s">
         <v>131</v>
       </c>
-      <c r="E47" s="17"/>
-      <c r="F47" s="17"/>
+      <c r="E47" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="F47" s="17" t="s">
+        <v>183</v>
+      </c>
       <c r="G47" s="18">
         <v>26</v>
       </c>
@@ -2666,8 +3116,12 @@
       <c r="D48" s="12" t="s">
         <v>132</v>
       </c>
-      <c r="E48" s="12"/>
-      <c r="F48" s="12"/>
+      <c r="E48" s="12" t="s">
+        <v>224</v>
+      </c>
+      <c r="F48" s="12" t="s">
+        <v>181</v>
+      </c>
       <c r="G48" s="13">
         <v>18</v>
       </c>
@@ -2698,8 +3152,12 @@
       <c r="D49" s="17" t="s">
         <v>133</v>
       </c>
-      <c r="E49" s="17"/>
-      <c r="F49" s="17"/>
+      <c r="E49" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="F49" s="17" t="s">
+        <v>181</v>
+      </c>
       <c r="G49" s="18">
         <v>8</v>
       </c>
@@ -2730,8 +3188,12 @@
       <c r="D50" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="E50" s="12"/>
-      <c r="F50" s="12"/>
+      <c r="E50" s="12" t="s">
+        <v>195</v>
+      </c>
+      <c r="F50" s="12" t="s">
+        <v>179</v>
+      </c>
       <c r="G50" s="13">
         <v>60</v>
       </c>
@@ -2762,8 +3224,12 @@
       <c r="D51" s="17" t="s">
         <v>134</v>
       </c>
-      <c r="E51" s="17"/>
-      <c r="F51" s="17"/>
+      <c r="E51" s="17" t="s">
+        <v>226</v>
+      </c>
+      <c r="F51" s="17" t="s">
+        <v>203</v>
+      </c>
       <c r="G51" s="18">
         <v>172</v>
       </c>
@@ -2794,8 +3260,12 @@
       <c r="D52" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="E52" s="12"/>
-      <c r="F52" s="12"/>
+      <c r="E52" s="12" t="s">
+        <v>198</v>
+      </c>
+      <c r="F52" s="12" t="s">
+        <v>177</v>
+      </c>
       <c r="G52" s="13">
         <v>8</v>
       </c>
@@ -2826,8 +3296,12 @@
       <c r="D53" s="17" t="s">
         <v>135</v>
       </c>
-      <c r="E53" s="17"/>
-      <c r="F53" s="17"/>
+      <c r="E53" s="17" t="s">
+        <v>227</v>
+      </c>
+      <c r="F53" s="17" t="s">
+        <v>187</v>
+      </c>
       <c r="G53" s="18">
         <v>86</v>
       </c>
@@ -2858,8 +3332,12 @@
       <c r="D54" s="12" t="s">
         <v>136</v>
       </c>
-      <c r="E54" s="12"/>
-      <c r="F54" s="12"/>
+      <c r="E54" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="F54" s="12" t="s">
+        <v>185</v>
+      </c>
       <c r="G54" s="13">
         <v>115</v>
       </c>
@@ -2890,8 +3368,12 @@
       <c r="D55" s="17" t="s">
         <v>109</v>
       </c>
-      <c r="E55" s="17"/>
-      <c r="F55" s="17"/>
+      <c r="E55" s="17" t="s">
+        <v>201</v>
+      </c>
+      <c r="F55" s="17" t="s">
+        <v>183</v>
+      </c>
       <c r="G55" s="18">
         <v>56</v>
       </c>
@@ -2922,8 +3404,12 @@
       <c r="D56" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="E56" s="12"/>
-      <c r="F56" s="12"/>
+      <c r="E56" s="12" t="s">
+        <v>202</v>
+      </c>
+      <c r="F56" s="12" t="s">
+        <v>203</v>
+      </c>
       <c r="G56" s="13">
         <v>45</v>
       </c>
@@ -2954,8 +3440,12 @@
       <c r="D57" s="17" t="s">
         <v>111</v>
       </c>
-      <c r="E57" s="17"/>
-      <c r="F57" s="17"/>
+      <c r="E57" s="17" t="s">
+        <v>204</v>
+      </c>
+      <c r="F57" s="17" t="s">
+        <v>187</v>
+      </c>
       <c r="G57" s="18">
         <v>19</v>
       </c>
@@ -2986,8 +3476,12 @@
       <c r="D58" s="12" t="s">
         <v>137</v>
       </c>
-      <c r="E58" s="12"/>
-      <c r="F58" s="12"/>
+      <c r="E58" s="12" t="s">
+        <v>229</v>
+      </c>
+      <c r="F58" s="12" t="s">
+        <v>197</v>
+      </c>
       <c r="G58" s="13">
         <v>34</v>
       </c>
@@ -3018,8 +3512,12 @@
       <c r="D59" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="E59" s="17"/>
-      <c r="F59" s="17"/>
+      <c r="E59" s="17" t="s">
+        <v>230</v>
+      </c>
+      <c r="F59" s="17" t="s">
+        <v>190</v>
+      </c>
       <c r="G59" s="18">
         <v>22</v>
       </c>
@@ -3050,8 +3548,12 @@
       <c r="D60" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="E60" s="12"/>
-      <c r="F60" s="12"/>
+      <c r="E60" s="12" t="s">
+        <v>210</v>
+      </c>
+      <c r="F60" s="12" t="s">
+        <v>197</v>
+      </c>
       <c r="G60" s="13">
         <v>68</v>
       </c>
@@ -3082,8 +3584,12 @@
       <c r="D61" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="E61" s="17"/>
-      <c r="F61" s="17"/>
+      <c r="E61" s="17" t="s">
+        <v>211</v>
+      </c>
+      <c r="F61" s="17" t="s">
+        <v>203</v>
+      </c>
       <c r="G61" s="18">
         <v>91</v>
       </c>
@@ -3114,8 +3620,12 @@
       <c r="D62" s="12" t="s">
         <v>139</v>
       </c>
-      <c r="E62" s="12"/>
-      <c r="F62" s="12"/>
+      <c r="E62" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="F62" s="12" t="s">
+        <v>177</v>
+      </c>
       <c r="G62" s="13">
         <v>19</v>
       </c>
@@ -3146,8 +3656,12 @@
       <c r="D63" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="E63" s="17"/>
-      <c r="F63" s="17"/>
+      <c r="E63" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="F63" s="17" t="s">
+        <v>190</v>
+      </c>
       <c r="G63" s="18">
         <v>31</v>
       </c>
@@ -3178,8 +3692,12 @@
       <c r="D64" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="E64" s="12"/>
-      <c r="F64" s="12"/>
+      <c r="E64" s="12" t="s">
+        <v>217</v>
+      </c>
+      <c r="F64" s="12" t="s">
+        <v>197</v>
+      </c>
       <c r="G64" s="13">
         <v>73</v>
       </c>
@@ -3210,8 +3728,12 @@
       <c r="D65" s="17" t="s">
         <v>140</v>
       </c>
-      <c r="E65" s="17"/>
-      <c r="F65" s="17"/>
+      <c r="E65" s="17" t="s">
+        <v>232</v>
+      </c>
+      <c r="F65" s="17" t="s">
+        <v>185</v>
+      </c>
       <c r="G65" s="18">
         <v>45</v>
       </c>
@@ -3242,8 +3764,12 @@
       <c r="D66" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="E66" s="12"/>
-      <c r="F66" s="12"/>
+      <c r="E66" s="12" t="s">
+        <v>218</v>
+      </c>
+      <c r="F66" s="12" t="s">
+        <v>190</v>
+      </c>
       <c r="G66" s="13">
         <v>1</v>
       </c>
@@ -3274,8 +3800,12 @@
       <c r="D67" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="E67" s="17"/>
-      <c r="F67" s="17"/>
+      <c r="E67" s="17" t="s">
+        <v>182</v>
+      </c>
+      <c r="F67" s="17" t="s">
+        <v>183</v>
+      </c>
       <c r="G67" s="18">
         <v>10</v>
       </c>
@@ -3306,8 +3836,12 @@
       <c r="D68" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="E68" s="12"/>
-      <c r="F68" s="12"/>
+      <c r="E68" s="12" t="s">
+        <v>233</v>
+      </c>
+      <c r="F68" s="12" t="s">
+        <v>183</v>
+      </c>
       <c r="G68" s="13">
         <v>18</v>
       </c>
@@ -3338,8 +3872,12 @@
       <c r="D69" s="17" t="s">
         <v>142</v>
       </c>
-      <c r="E69" s="17"/>
-      <c r="F69" s="17"/>
+      <c r="E69" s="17" t="s">
+        <v>234</v>
+      </c>
+      <c r="F69" s="17" t="s">
+        <v>183</v>
+      </c>
       <c r="G69" s="18">
         <v>2</v>
       </c>
@@ -3370,8 +3908,12 @@
       <c r="D70" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="E70" s="12"/>
-      <c r="F70" s="12"/>
+      <c r="E70" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="F70" s="12" t="s">
+        <v>190</v>
+      </c>
       <c r="G70" s="13">
         <v>21</v>
       </c>
@@ -3402,8 +3944,12 @@
       <c r="D71" s="17" t="s">
         <v>143</v>
       </c>
-      <c r="E71" s="17"/>
-      <c r="F71" s="17"/>
+      <c r="E71" s="17" t="s">
+        <v>235</v>
+      </c>
+      <c r="F71" s="17" t="s">
+        <v>181</v>
+      </c>
       <c r="G71" s="18">
         <v>46</v>
       </c>
@@ -3434,8 +3980,12 @@
       <c r="D72" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="E72" s="12"/>
-      <c r="F72" s="12"/>
+      <c r="E72" s="12" t="s">
+        <v>223</v>
+      </c>
+      <c r="F72" s="12" t="s">
+        <v>183</v>
+      </c>
       <c r="G72" s="13">
         <v>26</v>
       </c>
@@ -3466,8 +4016,12 @@
       <c r="D73" s="17" t="s">
         <v>133</v>
       </c>
-      <c r="E73" s="17"/>
-      <c r="F73" s="17"/>
+      <c r="E73" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="F73" s="17" t="s">
+        <v>181</v>
+      </c>
       <c r="G73" s="18">
         <v>8</v>
       </c>
@@ -3498,8 +4052,12 @@
       <c r="D74" s="12" t="s">
         <v>135</v>
       </c>
-      <c r="E74" s="12"/>
-      <c r="F74" s="12"/>
+      <c r="E74" s="12" t="s">
+        <v>227</v>
+      </c>
+      <c r="F74" s="12" t="s">
+        <v>187</v>
+      </c>
       <c r="G74" s="13">
         <v>86</v>
       </c>
@@ -3530,8 +4088,12 @@
       <c r="D75" s="17" t="s">
         <v>111</v>
       </c>
-      <c r="E75" s="17"/>
-      <c r="F75" s="17"/>
+      <c r="E75" s="17" t="s">
+        <v>204</v>
+      </c>
+      <c r="F75" s="17" t="s">
+        <v>187</v>
+      </c>
       <c r="G75" s="18">
         <v>17</v>
       </c>
@@ -3562,8 +4124,12 @@
       <c r="D76" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="E76" s="12"/>
-      <c r="F76" s="12"/>
+      <c r="E76" s="12" t="s">
+        <v>206</v>
+      </c>
+      <c r="F76" s="12" t="s">
+        <v>185</v>
+      </c>
       <c r="G76" s="13">
         <v>53</v>
       </c>
@@ -3594,8 +4160,12 @@
       <c r="D77" s="17" t="s">
         <v>144</v>
       </c>
-      <c r="E77" s="17"/>
-      <c r="F77" s="17"/>
+      <c r="E77" s="17" t="s">
+        <v>236</v>
+      </c>
+      <c r="F77" s="17" t="s">
+        <v>190</v>
+      </c>
       <c r="G77" s="18">
         <v>75</v>
       </c>
@@ -3626,8 +4196,12 @@
       <c r="D78" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="E78" s="12"/>
-      <c r="F78" s="12"/>
+      <c r="E78" s="12" t="s">
+        <v>215</v>
+      </c>
+      <c r="F78" s="12" t="s">
+        <v>179</v>
+      </c>
       <c r="G78" s="13">
         <v>14</v>
       </c>
@@ -3658,8 +4232,12 @@
       <c r="D79" s="17" t="s">
         <v>142</v>
       </c>
-      <c r="E79" s="17"/>
-      <c r="F79" s="17"/>
+      <c r="E79" s="17" t="s">
+        <v>217</v>
+      </c>
+      <c r="F79" s="17" t="s">
+        <v>197</v>
+      </c>
       <c r="G79" s="18">
         <v>2</v>
       </c>
@@ -3690,8 +4268,12 @@
       <c r="D80" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="E80" s="12"/>
-      <c r="F80" s="12"/>
+      <c r="E80" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="F80" s="12" t="s">
+        <v>177</v>
+      </c>
       <c r="G80" s="13">
         <v>31</v>
       </c>
@@ -3722,8 +4304,12 @@
       <c r="D81" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="E81" s="17"/>
-      <c r="F81" s="17"/>
+      <c r="E81" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="F81" s="17" t="s">
+        <v>179</v>
+      </c>
       <c r="G81" s="18">
         <v>40</v>
       </c>
@@ -3754,8 +4340,12 @@
       <c r="D82" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="E82" s="12"/>
-      <c r="F82" s="12"/>
+      <c r="E82" s="12" t="s">
+        <v>218</v>
+      </c>
+      <c r="F82" s="12" t="s">
+        <v>190</v>
+      </c>
       <c r="G82" s="13">
         <v>33</v>
       </c>
@@ -3786,8 +4376,12 @@
       <c r="D83" s="17" t="s">
         <v>107</v>
       </c>
-      <c r="E83" s="17"/>
-      <c r="F83" s="17"/>
+      <c r="E83" s="17" t="s">
+        <v>237</v>
+      </c>
+      <c r="F83" s="17" t="s">
+        <v>190</v>
+      </c>
       <c r="G83" s="18">
         <v>4</v>
       </c>
@@ -3818,8 +4412,12 @@
       <c r="D84" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="E84" s="12"/>
-      <c r="F84" s="12"/>
+      <c r="E84" s="12" t="s">
+        <v>233</v>
+      </c>
+      <c r="F84" s="12" t="s">
+        <v>183</v>
+      </c>
       <c r="G84" s="13">
         <v>34</v>
       </c>
@@ -3850,8 +4448,12 @@
       <c r="D85" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="E85" s="17"/>
-      <c r="F85" s="17"/>
+      <c r="E85" s="17" t="s">
+        <v>234</v>
+      </c>
+      <c r="F85" s="17" t="s">
+        <v>183</v>
+      </c>
       <c r="G85" s="18">
         <v>110</v>
       </c>
@@ -3882,8 +4484,12 @@
       <c r="D86" s="12" t="s">
         <v>144</v>
       </c>
-      <c r="E86" s="12"/>
-      <c r="F86" s="12"/>
+      <c r="E86" s="12" t="s">
+        <v>238</v>
+      </c>
+      <c r="F86" s="12" t="s">
+        <v>183</v>
+      </c>
       <c r="G86" s="13">
         <v>68</v>
       </c>
@@ -3914,8 +4520,12 @@
       <c r="D87" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="E87" s="17"/>
-      <c r="F87" s="17"/>
+      <c r="E87" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="F87" s="17" t="s">
+        <v>183</v>
+      </c>
       <c r="G87" s="18">
         <v>8</v>
       </c>
@@ -3946,8 +4556,12 @@
       <c r="D88" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="E88" s="12"/>
-      <c r="F88" s="12"/>
+      <c r="E88" s="12" t="s">
+        <v>193</v>
+      </c>
+      <c r="F88" s="12" t="s">
+        <v>179</v>
+      </c>
       <c r="G88" s="13">
         <v>1</v>
       </c>
@@ -3978,8 +4592,12 @@
       <c r="D89" s="17" t="s">
         <v>145</v>
       </c>
-      <c r="E89" s="17"/>
-      <c r="F89" s="17"/>
+      <c r="E89" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="F89" s="17" t="s">
+        <v>197</v>
+      </c>
       <c r="G89" s="18">
         <v>22</v>
       </c>
@@ -4010,8 +4628,12 @@
       <c r="D90" s="12" t="s">
         <v>146</v>
       </c>
-      <c r="E90" s="12"/>
-      <c r="F90" s="12"/>
+      <c r="E90" s="12" t="s">
+        <v>239</v>
+      </c>
+      <c r="F90" s="12" t="s">
+        <v>177</v>
+      </c>
       <c r="G90" s="13">
         <v>41</v>
       </c>
@@ -4042,8 +4664,12 @@
       <c r="D91" s="17" t="s">
         <v>131</v>
       </c>
-      <c r="E91" s="17"/>
-      <c r="F91" s="17"/>
+      <c r="E91" s="17" t="s">
+        <v>199</v>
+      </c>
+      <c r="F91" s="17" t="s">
+        <v>177</v>
+      </c>
       <c r="G91" s="18">
         <v>20</v>
       </c>
@@ -4074,8 +4700,12 @@
       <c r="D92" s="12" t="s">
         <v>147</v>
       </c>
-      <c r="E92" s="12"/>
-      <c r="F92" s="12"/>
+      <c r="E92" s="12" t="s">
+        <v>200</v>
+      </c>
+      <c r="F92" s="12" t="s">
+        <v>185</v>
+      </c>
       <c r="G92" s="13">
         <v>28</v>
       </c>
@@ -4106,8 +4736,12 @@
       <c r="D93" s="17" t="s">
         <v>124</v>
       </c>
-      <c r="E93" s="17"/>
-      <c r="F93" s="17"/>
+      <c r="E93" s="17" t="s">
+        <v>240</v>
+      </c>
+      <c r="F93" s="17" t="s">
+        <v>177</v>
+      </c>
       <c r="G93" s="18">
         <v>62</v>
       </c>
@@ -4138,8 +4772,12 @@
       <c r="D94" s="12" t="s">
         <v>148</v>
       </c>
-      <c r="E94" s="12"/>
-      <c r="F94" s="12"/>
+      <c r="E94" s="12" t="s">
+        <v>236</v>
+      </c>
+      <c r="F94" s="12" t="s">
+        <v>190</v>
+      </c>
       <c r="G94" s="13">
         <v>21</v>
       </c>
@@ -4170,8 +4808,12 @@
       <c r="D95" s="17" t="s">
         <v>149</v>
       </c>
-      <c r="E95" s="17"/>
-      <c r="F95" s="17"/>
+      <c r="E95" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="F95" s="17" t="s">
+        <v>179</v>
+      </c>
       <c r="G95" s="18">
         <v>56</v>
       </c>
@@ -4202,8 +4844,12 @@
       <c r="D96" s="12" t="s">
         <v>150</v>
       </c>
-      <c r="E96" s="12"/>
-      <c r="F96" s="12"/>
+      <c r="E96" s="12" t="s">
+        <v>242</v>
+      </c>
+      <c r="F96" s="12" t="s">
+        <v>185</v>
+      </c>
       <c r="G96" s="13">
         <v>32</v>
       </c>
@@ -4234,8 +4880,12 @@
       <c r="D97" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="E97" s="17"/>
-      <c r="F97" s="17"/>
+      <c r="E97" s="17" t="s">
+        <v>216</v>
+      </c>
+      <c r="F97" s="17" t="s">
+        <v>187</v>
+      </c>
       <c r="G97" s="18">
         <v>8</v>
       </c>
@@ -4266,8 +4916,12 @@
       <c r="D98" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="E98" s="12"/>
-      <c r="F98" s="12"/>
+      <c r="E98" s="12" t="s">
+        <v>217</v>
+      </c>
+      <c r="F98" s="12" t="s">
+        <v>197</v>
+      </c>
       <c r="G98" s="13">
         <v>52</v>
       </c>
@@ -4298,8 +4952,12 @@
       <c r="D99" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="E99" s="17"/>
-      <c r="F99" s="17"/>
+      <c r="E99" s="17" t="s">
+        <v>217</v>
+      </c>
+      <c r="F99" s="17" t="s">
+        <v>197</v>
+      </c>
       <c r="G99" s="18">
         <v>28</v>
       </c>
@@ -4330,8 +4988,12 @@
       <c r="D100" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="E100" s="12"/>
-      <c r="F100" s="12"/>
+      <c r="E100" s="12" t="s">
+        <v>232</v>
+      </c>
+      <c r="F100" s="12" t="s">
+        <v>185</v>
+      </c>
       <c r="G100" s="13">
         <v>84</v>
       </c>
@@ -4362,8 +5024,12 @@
       <c r="D101" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="E101" s="17"/>
-      <c r="F101" s="17"/>
+      <c r="E101" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="F101" s="17" t="s">
+        <v>179</v>
+      </c>
       <c r="G101" s="18">
         <v>18</v>
       </c>
@@ -4394,8 +5060,12 @@
       <c r="D102" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="E102" s="12"/>
-      <c r="F102" s="12"/>
+      <c r="E102" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="F102" s="12" t="s">
+        <v>179</v>
+      </c>
       <c r="G102" s="13">
         <v>28</v>
       </c>
@@ -4426,8 +5096,12 @@
       <c r="D103" s="17" t="s">
         <v>111</v>
       </c>
-      <c r="E103" s="17"/>
-      <c r="F103" s="17"/>
+      <c r="E103" s="17" t="s">
+        <v>218</v>
+      </c>
+      <c r="F103" s="17" t="s">
+        <v>190</v>
+      </c>
       <c r="G103" s="18">
         <v>17</v>
       </c>
@@ -4458,8 +5132,12 @@
       <c r="D104" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="E104" s="12"/>
-      <c r="F104" s="12"/>
+      <c r="E104" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="F104" s="12" t="s">
+        <v>181</v>
+      </c>
       <c r="G104" s="13">
         <v>110</v>
       </c>
@@ -4490,8 +5168,12 @@
       <c r="D105" s="17" t="s">
         <v>114</v>
       </c>
-      <c r="E105" s="17"/>
-      <c r="F105" s="17"/>
+      <c r="E105" s="17" t="s">
+        <v>243</v>
+      </c>
+      <c r="F105" s="17" t="s">
+        <v>181</v>
+      </c>
       <c r="G105" s="18">
         <v>23</v>
       </c>
@@ -4522,8 +5204,12 @@
       <c r="D106" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="E106" s="12"/>
-      <c r="F106" s="12"/>
+      <c r="E106" s="12" t="s">
+        <v>244</v>
+      </c>
+      <c r="F106" s="12" t="s">
+        <v>190</v>
+      </c>
       <c r="G106" s="13">
         <v>38</v>
       </c>
@@ -4554,8 +5240,12 @@
       <c r="D107" s="17" t="s">
         <v>116</v>
       </c>
-      <c r="E107" s="17"/>
-      <c r="F107" s="17"/>
+      <c r="E107" s="17" t="s">
+        <v>245</v>
+      </c>
+      <c r="F107" s="17" t="s">
+        <v>246</v>
+      </c>
       <c r="G107" s="18">
         <v>6</v>
       </c>
@@ -4586,8 +5276,12 @@
       <c r="D108" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="E108" s="12"/>
-      <c r="F108" s="12"/>
+      <c r="E108" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="F108" s="12" t="s">
+        <v>179</v>
+      </c>
       <c r="G108" s="13">
         <v>80</v>
       </c>
@@ -4618,8 +5312,12 @@
       <c r="D109" s="17" t="s">
         <v>120</v>
       </c>
-      <c r="E109" s="17"/>
-      <c r="F109" s="17"/>
+      <c r="E109" s="17" t="s">
+        <v>237</v>
+      </c>
+      <c r="F109" s="17" t="s">
+        <v>190</v>
+      </c>
       <c r="G109" s="18">
         <v>58</v>
       </c>
@@ -4650,8 +5348,12 @@
       <c r="D110" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="E110" s="12"/>
-      <c r="F110" s="12"/>
+      <c r="E110" s="12" t="s">
+        <v>219</v>
+      </c>
+      <c r="F110" s="12" t="s">
+        <v>185</v>
+      </c>
       <c r="G110" s="13">
         <v>13</v>
       </c>
@@ -4682,8 +5384,12 @@
       <c r="D111" s="17" t="s">
         <v>124</v>
       </c>
-      <c r="E111" s="17"/>
-      <c r="F111" s="17"/>
+      <c r="E111" s="17" t="s">
+        <v>219</v>
+      </c>
+      <c r="F111" s="17" t="s">
+        <v>185</v>
+      </c>
       <c r="G111" s="18">
         <v>62</v>
       </c>
@@ -4714,8 +5420,12 @@
       <c r="D112" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="E112" s="12"/>
-      <c r="F112" s="12"/>
+      <c r="E112" s="12" t="s">
+        <v>233</v>
+      </c>
+      <c r="F112" s="12" t="s">
+        <v>183</v>
+      </c>
       <c r="G112" s="13">
         <v>1</v>
       </c>
@@ -4746,8 +5456,12 @@
       <c r="D113" s="17" t="s">
         <v>127</v>
       </c>
-      <c r="E113" s="17"/>
-      <c r="F113" s="17"/>
+      <c r="E113" s="17" t="s">
+        <v>234</v>
+      </c>
+      <c r="F113" s="17" t="s">
+        <v>183</v>
+      </c>
       <c r="G113" s="18">
         <v>60</v>
       </c>
@@ -4778,8 +5492,12 @@
       <c r="D114" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="E114" s="12"/>
-      <c r="F114" s="12"/>
+      <c r="E114" s="12" t="s">
+        <v>238</v>
+      </c>
+      <c r="F114" s="12" t="s">
+        <v>183</v>
+      </c>
       <c r="G114" s="13">
         <v>101</v>
       </c>
@@ -4810,8 +5528,12 @@
       <c r="D115" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="E115" s="17"/>
-      <c r="F115" s="17"/>
+      <c r="E115" s="17" t="s">
+        <v>220</v>
+      </c>
+      <c r="F115" s="17" t="s">
+        <v>177</v>
+      </c>
       <c r="G115" s="18">
         <v>22</v>
       </c>
@@ -4842,8 +5564,12 @@
       <c r="D116" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="E116" s="12"/>
-      <c r="F116" s="12"/>
+      <c r="E116" s="12" t="s">
+        <v>222</v>
+      </c>
+      <c r="F116" s="12" t="s">
+        <v>179</v>
+      </c>
       <c r="G116" s="13">
         <v>20</v>
       </c>
@@ -4874,8 +5600,12 @@
       <c r="D117" s="17" t="s">
         <v>132</v>
       </c>
-      <c r="E117" s="17"/>
-      <c r="F117" s="17"/>
+      <c r="E117" s="17" t="s">
+        <v>235</v>
+      </c>
+      <c r="F117" s="17" t="s">
+        <v>181</v>
+      </c>
       <c r="G117" s="18">
         <v>18</v>
       </c>
@@ -4906,8 +5636,12 @@
       <c r="D118" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="E118" s="12"/>
-      <c r="F118" s="12"/>
+      <c r="E118" s="12" t="s">
+        <v>223</v>
+      </c>
+      <c r="F118" s="12" t="s">
+        <v>183</v>
+      </c>
       <c r="G118" s="13">
         <v>172</v>
       </c>
@@ -4938,8 +5672,12 @@
       <c r="D119" s="17" t="s">
         <v>136</v>
       </c>
-      <c r="E119" s="17"/>
-      <c r="F119" s="17"/>
+      <c r="E119" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="F119" s="17" t="s">
+        <v>183</v>
+      </c>
       <c r="G119" s="18">
         <v>115</v>
       </c>
@@ -4970,8 +5708,12 @@
       <c r="D120" s="12" t="s">
         <v>137</v>
       </c>
-      <c r="E120" s="12"/>
-      <c r="F120" s="12"/>
+      <c r="E120" s="12" t="s">
+        <v>193</v>
+      </c>
+      <c r="F120" s="12" t="s">
+        <v>179</v>
+      </c>
       <c r="G120" s="13">
         <v>34</v>
       </c>
@@ -5002,8 +5744,12 @@
       <c r="D121" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="E121" s="17"/>
-      <c r="F121" s="17"/>
+      <c r="E121" s="17" t="s">
+        <v>193</v>
+      </c>
+      <c r="F121" s="17" t="s">
+        <v>179</v>
+      </c>
       <c r="G121" s="18">
         <v>22</v>
       </c>
@@ -5034,8 +5780,12 @@
       <c r="D122" s="12" t="s">
         <v>139</v>
       </c>
-      <c r="E122" s="12"/>
-      <c r="F122" s="12"/>
+      <c r="E122" s="12" t="s">
+        <v>224</v>
+      </c>
+      <c r="F122" s="12" t="s">
+        <v>181</v>
+      </c>
       <c r="G122" s="13">
         <v>19</v>
       </c>
@@ -5066,8 +5816,12 @@
       <c r="D123" s="17" t="s">
         <v>140</v>
       </c>
-      <c r="E123" s="17"/>
-      <c r="F123" s="17"/>
+      <c r="E123" s="17" t="s">
+        <v>224</v>
+      </c>
+      <c r="F123" s="17" t="s">
+        <v>181</v>
+      </c>
       <c r="G123" s="18">
         <v>45</v>
       </c>
@@ -5098,8 +5852,12 @@
       <c r="D124" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="E124" s="12"/>
-      <c r="F124" s="12"/>
+      <c r="E124" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="F124" s="12" t="s">
+        <v>187</v>
+      </c>
       <c r="G124" s="13">
         <v>4</v>
       </c>
@@ -5130,8 +5888,12 @@
       <c r="D125" s="17" t="s">
         <v>143</v>
       </c>
-      <c r="E125" s="17"/>
-      <c r="F125" s="17"/>
+      <c r="E125" s="17" t="s">
+        <v>194</v>
+      </c>
+      <c r="F125" s="17" t="s">
+        <v>187</v>
+      </c>
       <c r="G125" s="18">
         <v>46</v>
       </c>
@@ -5162,8 +5924,12 @@
       <c r="D126" s="12" t="s">
         <v>144</v>
       </c>
-      <c r="E126" s="12"/>
-      <c r="F126" s="12"/>
+      <c r="E126" s="12" t="s">
+        <v>248</v>
+      </c>
+      <c r="F126" s="12" t="s">
+        <v>246</v>
+      </c>
       <c r="G126" s="13">
         <v>7</v>
       </c>
@@ -5194,8 +5960,12 @@
       <c r="D127" s="17" t="s">
         <v>145</v>
       </c>
-      <c r="E127" s="17"/>
-      <c r="F127" s="17"/>
+      <c r="E127" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="F127" s="17" t="s">
+        <v>197</v>
+      </c>
       <c r="G127" s="18">
         <v>22</v>
       </c>
@@ -5226,8 +5996,12 @@
       <c r="D128" s="12" t="s">
         <v>146</v>
       </c>
-      <c r="E128" s="12"/>
-      <c r="F128" s="12"/>
+      <c r="E128" s="12" t="s">
+        <v>226</v>
+      </c>
+      <c r="F128" s="12" t="s">
+        <v>203</v>
+      </c>
       <c r="G128" s="13">
         <v>41</v>
       </c>
@@ -5258,8 +6032,12 @@
       <c r="D129" s="17" t="s">
         <v>147</v>
       </c>
-      <c r="E129" s="17"/>
-      <c r="F129" s="17"/>
+      <c r="E129" s="17" t="s">
+        <v>226</v>
+      </c>
+      <c r="F129" s="17" t="s">
+        <v>203</v>
+      </c>
       <c r="G129" s="18">
         <v>28</v>
       </c>
@@ -5290,8 +6068,12 @@
       <c r="D130" s="12" t="s">
         <v>148</v>
       </c>
-      <c r="E130" s="12"/>
-      <c r="F130" s="12"/>
+      <c r="E130" s="12" t="s">
+        <v>239</v>
+      </c>
+      <c r="F130" s="12" t="s">
+        <v>177</v>
+      </c>
       <c r="G130" s="13">
         <v>21</v>
       </c>
@@ -5322,8 +6104,12 @@
       <c r="D131" s="17" t="s">
         <v>149</v>
       </c>
-      <c r="E131" s="17"/>
-      <c r="F131" s="17"/>
+      <c r="E131" s="17" t="s">
+        <v>239</v>
+      </c>
+      <c r="F131" s="17" t="s">
+        <v>177</v>
+      </c>
       <c r="G131" s="18">
         <v>56</v>
       </c>
@@ -5354,8 +6140,12 @@
       <c r="D132" s="12" t="s">
         <v>150</v>
       </c>
-      <c r="E132" s="12"/>
-      <c r="F132" s="12"/>
+      <c r="E132" s="12" t="s">
+        <v>199</v>
+      </c>
+      <c r="F132" s="12" t="s">
+        <v>177</v>
+      </c>
       <c r="G132" s="13">
         <v>32</v>
       </c>
@@ -5386,8 +6176,12 @@
       <c r="D133" s="17" t="s">
         <v>127</v>
       </c>
-      <c r="E133" s="17"/>
-      <c r="F133" s="17"/>
+      <c r="E133" s="17" t="s">
+        <v>228</v>
+      </c>
+      <c r="F133" s="17" t="s">
+        <v>185</v>
+      </c>
       <c r="G133" s="18">
         <v>20</v>
       </c>
@@ -5418,8 +6212,12 @@
       <c r="D134" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="E134" s="12"/>
-      <c r="F134" s="12"/>
+      <c r="E134" s="12" t="s">
+        <v>249</v>
+      </c>
+      <c r="F134" s="12" t="s">
+        <v>190</v>
+      </c>
       <c r="G134" s="13">
         <v>20</v>
       </c>
@@ -5450,8 +6248,12 @@
       <c r="D135" s="17" t="s">
         <v>151</v>
       </c>
-      <c r="E135" s="17"/>
-      <c r="F135" s="17"/>
+      <c r="E135" s="17" t="s">
+        <v>200</v>
+      </c>
+      <c r="F135" s="17" t="s">
+        <v>185</v>
+      </c>
       <c r="G135" s="18">
         <v>24</v>
       </c>
@@ -5482,8 +6284,12 @@
       <c r="D136" s="12" t="s">
         <v>152</v>
       </c>
-      <c r="E136" s="12"/>
-      <c r="F136" s="12"/>
+      <c r="E136" s="12" t="s">
+        <v>202</v>
+      </c>
+      <c r="F136" s="12" t="s">
+        <v>203</v>
+      </c>
       <c r="G136" s="13">
         <v>22</v>
       </c>
@@ -5514,8 +6320,12 @@
       <c r="D137" s="17" t="s">
         <v>111</v>
       </c>
-      <c r="E137" s="17"/>
-      <c r="F137" s="17"/>
+      <c r="E137" s="17" t="s">
+        <v>204</v>
+      </c>
+      <c r="F137" s="17" t="s">
+        <v>187</v>
+      </c>
       <c r="G137" s="18">
         <v>12</v>
       </c>
@@ -5546,8 +6356,12 @@
       <c r="D138" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="E138" s="12"/>
-      <c r="F138" s="12"/>
+      <c r="E138" s="12" t="s">
+        <v>204</v>
+      </c>
+      <c r="F138" s="12" t="s">
+        <v>187</v>
+      </c>
       <c r="G138" s="13">
         <v>52</v>
       </c>
@@ -5578,8 +6392,12 @@
       <c r="D139" s="17" t="s">
         <v>131</v>
       </c>
-      <c r="E139" s="17"/>
-      <c r="F139" s="17"/>
+      <c r="E139" s="17" t="s">
+        <v>205</v>
+      </c>
+      <c r="F139" s="17" t="s">
+        <v>183</v>
+      </c>
       <c r="G139" s="18">
         <v>15</v>
       </c>
@@ -5610,8 +6428,12 @@
       <c r="D140" s="12" t="s">
         <v>142</v>
       </c>
-      <c r="E140" s="12"/>
-      <c r="F140" s="12"/>
+      <c r="E140" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="F140" s="12" t="s">
+        <v>183</v>
+      </c>
       <c r="G140" s="13">
         <v>1</v>
       </c>
@@ -5642,8 +6464,12 @@
       <c r="D141" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="E141" s="17"/>
-      <c r="F141" s="17"/>
+      <c r="E141" s="17" t="s">
+        <v>250</v>
+      </c>
+      <c r="F141" s="17" t="s">
+        <v>179</v>
+      </c>
       <c r="G141" s="18">
         <v>45</v>
       </c>
@@ -5674,8 +6500,12 @@
       <c r="D142" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="E142" s="12"/>
-      <c r="F142" s="12"/>
+      <c r="E142" s="12" t="s">
+        <v>229</v>
+      </c>
+      <c r="F142" s="12" t="s">
+        <v>197</v>
+      </c>
       <c r="G142" s="13">
         <v>25</v>
       </c>
@@ -5706,8 +6536,12 @@
       <c r="D143" s="17" t="s">
         <v>153</v>
       </c>
-      <c r="E143" s="17"/>
-      <c r="F143" s="17"/>
+      <c r="E143" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="F143" s="17" t="s">
+        <v>190</v>
+      </c>
       <c r="G143" s="18">
         <v>47</v>
       </c>
@@ -5738,8 +6572,12 @@
       <c r="D144" s="12" t="s">
         <v>154</v>
       </c>
-      <c r="E144" s="12"/>
-      <c r="F144" s="12"/>
+      <c r="E144" s="12" t="s">
+        <v>230</v>
+      </c>
+      <c r="F144" s="12" t="s">
+        <v>190</v>
+      </c>
       <c r="G144" s="13">
         <v>13</v>
       </c>
@@ -5770,8 +6608,12 @@
       <c r="D145" s="17" t="s">
         <v>149</v>
       </c>
-      <c r="E145" s="17"/>
-      <c r="F145" s="17"/>
+      <c r="E145" s="17" t="s">
+        <v>230</v>
+      </c>
+      <c r="F145" s="17" t="s">
+        <v>190</v>
+      </c>
       <c r="G145" s="18">
         <v>31</v>
       </c>
@@ -5802,8 +6644,12 @@
       <c r="D146" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="E146" s="12"/>
-      <c r="F146" s="12"/>
+      <c r="E146" s="12" t="s">
+        <v>240</v>
+      </c>
+      <c r="F146" s="12" t="s">
+        <v>177</v>
+      </c>
       <c r="G146" s="13">
         <v>4</v>
       </c>
@@ -5834,8 +6680,12 @@
       <c r="D147" s="17" t="s">
         <v>155</v>
       </c>
-      <c r="E147" s="17"/>
-      <c r="F147" s="17"/>
+      <c r="E147" s="17" t="s">
+        <v>236</v>
+      </c>
+      <c r="F147" s="17" t="s">
+        <v>190</v>
+      </c>
       <c r="G147" s="18">
         <v>50</v>
       </c>
@@ -5866,8 +6716,12 @@
       <c r="D148" s="12" t="s">
         <v>132</v>
       </c>
-      <c r="E148" s="12"/>
-      <c r="F148" s="12"/>
+      <c r="E148" s="12" t="s">
+        <v>236</v>
+      </c>
+      <c r="F148" s="12" t="s">
+        <v>190</v>
+      </c>
       <c r="G148" s="13">
         <v>11</v>
       </c>
@@ -5898,8 +6752,12 @@
       <c r="D149" s="17" t="s">
         <v>124</v>
       </c>
-      <c r="E149" s="17"/>
-      <c r="F149" s="17"/>
+      <c r="E149" s="17" t="s">
+        <v>208</v>
+      </c>
+      <c r="F149" s="17" t="s">
+        <v>203</v>
+      </c>
       <c r="G149" s="18">
         <v>52</v>
       </c>
@@ -5930,8 +6788,12 @@
       <c r="D150" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="E150" s="12"/>
-      <c r="F150" s="12"/>
+      <c r="E150" s="12" t="s">
+        <v>208</v>
+      </c>
+      <c r="F150" s="12" t="s">
+        <v>203</v>
+      </c>
       <c r="G150" s="13">
         <v>32</v>
       </c>
@@ -5962,8 +6824,12 @@
       <c r="D151" s="17" t="s">
         <v>156</v>
       </c>
-      <c r="E151" s="17"/>
-      <c r="F151" s="17"/>
+      <c r="E151" s="17" t="s">
+        <v>251</v>
+      </c>
+      <c r="F151" s="17" t="s">
+        <v>190</v>
+      </c>
       <c r="G151" s="18">
         <v>117</v>
       </c>
@@ -5994,8 +6860,12 @@
       <c r="D152" s="12" t="s">
         <v>157</v>
       </c>
-      <c r="E152" s="12"/>
-      <c r="F152" s="12"/>
+      <c r="E152" s="12" t="s">
+        <v>209</v>
+      </c>
+      <c r="F152" s="12" t="s">
+        <v>203</v>
+      </c>
       <c r="G152" s="13">
         <v>111</v>
       </c>
@@ -6026,8 +6896,12 @@
       <c r="D153" s="17" t="s">
         <v>144</v>
       </c>
-      <c r="E153" s="17"/>
-      <c r="F153" s="17"/>
+      <c r="E153" s="17" t="s">
+        <v>209</v>
+      </c>
+      <c r="F153" s="17" t="s">
+        <v>203</v>
+      </c>
       <c r="G153" s="18">
         <v>48</v>
       </c>
@@ -6058,8 +6932,12 @@
       <c r="D154" s="12" t="s">
         <v>158</v>
       </c>
-      <c r="E154" s="12"/>
-      <c r="F154" s="12"/>
+      <c r="E154" s="12" t="s">
+        <v>211</v>
+      </c>
+      <c r="F154" s="12" t="s">
+        <v>203</v>
+      </c>
       <c r="G154" s="13">
         <v>9</v>
       </c>
@@ -6090,8 +6968,12 @@
       <c r="D155" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="E155" s="17"/>
-      <c r="F155" s="17"/>
+      <c r="E155" s="17" t="s">
+        <v>231</v>
+      </c>
+      <c r="F155" s="17" t="s">
+        <v>177</v>
+      </c>
       <c r="G155" s="18">
         <v>12</v>
       </c>
@@ -6122,8 +7004,12 @@
       <c r="D156" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="E156" s="12"/>
-      <c r="F156" s="12"/>
+      <c r="E156" s="12" t="s">
+        <v>241</v>
+      </c>
+      <c r="F156" s="12" t="s">
+        <v>179</v>
+      </c>
       <c r="G156" s="13">
         <v>3</v>
       </c>
@@ -6154,8 +7040,12 @@
       <c r="D157" s="17" t="s">
         <v>147</v>
       </c>
-      <c r="E157" s="17"/>
-      <c r="F157" s="17"/>
+      <c r="E157" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="F157" s="17" t="s">
+        <v>179</v>
+      </c>
       <c r="G157" s="18">
         <v>21</v>
       </c>
@@ -6186,8 +7076,12 @@
       <c r="D158" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="E158" s="12"/>
-      <c r="F158" s="12"/>
+      <c r="E158" s="12" t="s">
+        <v>212</v>
+      </c>
+      <c r="F158" s="12" t="s">
+        <v>185</v>
+      </c>
       <c r="G158" s="13">
         <v>105</v>
       </c>
@@ -6218,8 +7112,12 @@
       <c r="D159" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="E159" s="17"/>
-      <c r="F159" s="17"/>
+      <c r="E159" s="17" t="s">
+        <v>212</v>
+      </c>
+      <c r="F159" s="17" t="s">
+        <v>185</v>
+      </c>
       <c r="G159" s="18">
         <v>51</v>
       </c>
@@ -6250,8 +7148,12 @@
       <c r="D160" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="E160" s="12"/>
-      <c r="F160" s="12"/>
+      <c r="E160" s="12" t="s">
+        <v>213</v>
+      </c>
+      <c r="F160" s="12" t="s">
+        <v>197</v>
+      </c>
       <c r="G160" s="13">
         <v>26</v>
       </c>
@@ -6282,8 +7184,12 @@
       <c r="D161" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="E161" s="17"/>
-      <c r="F161" s="17"/>
+      <c r="E161" s="17" t="s">
+        <v>213</v>
+      </c>
+      <c r="F161" s="17" t="s">
+        <v>197</v>
+      </c>
       <c r="G161" s="18">
         <v>14</v>
       </c>
@@ -6314,8 +7220,12 @@
       <c r="D162" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="E162" s="12"/>
-      <c r="F162" s="12"/>
+      <c r="E162" s="12" t="s">
+        <v>242</v>
+      </c>
+      <c r="F162" s="12" t="s">
+        <v>185</v>
+      </c>
       <c r="G162" s="13">
         <v>2</v>
       </c>
@@ -6346,8 +7256,12 @@
       <c r="D163" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="E163" s="17"/>
-      <c r="F163" s="17"/>
+      <c r="E163" s="17" t="s">
+        <v>252</v>
+      </c>
+      <c r="F163" s="17" t="s">
+        <v>177</v>
+      </c>
       <c r="G163" s="18">
         <v>4</v>
       </c>
@@ -6378,8 +7292,12 @@
       <c r="D164" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="E164" s="12"/>
-      <c r="F164" s="12"/>
+      <c r="E164" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="F164" s="12" t="s">
+        <v>190</v>
+      </c>
       <c r="G164" s="13">
         <v>20</v>
       </c>
@@ -6410,8 +7328,12 @@
       <c r="D165" s="17" t="s">
         <v>159</v>
       </c>
-      <c r="E165" s="17"/>
-      <c r="F165" s="17"/>
+      <c r="E165" s="17" t="s">
+        <v>254</v>
+      </c>
+      <c r="F165" s="17" t="s">
+        <v>183</v>
+      </c>
       <c r="G165" s="18">
         <v>16</v>
       </c>
@@ -6442,8 +7364,12 @@
       <c r="D166" s="12" t="s">
         <v>160</v>
       </c>
-      <c r="E166" s="12"/>
-      <c r="F166" s="12"/>
+      <c r="E166" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="F166" s="12" t="s">
+        <v>179</v>
+      </c>
       <c r="G166" s="13">
         <v>12</v>
       </c>
@@ -6474,8 +7400,12 @@
       <c r="D167" s="17" t="s">
         <v>161</v>
       </c>
-      <c r="E167" s="17"/>
-      <c r="F167" s="17"/>
+      <c r="E167" s="17" t="s">
+        <v>245</v>
+      </c>
+      <c r="F167" s="17" t="s">
+        <v>246</v>
+      </c>
       <c r="G167" s="21">
         <v>13</v>
       </c>
@@ -6506,8 +7436,12 @@
       <c r="D168" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="E168" s="12"/>
-      <c r="F168" s="12"/>
+      <c r="E168" s="12" t="s">
+        <v>248</v>
+      </c>
+      <c r="F168" s="12" t="s">
+        <v>246</v>
+      </c>
       <c r="G168" s="13">
         <v>14</v>
       </c>
@@ -6538,8 +7472,12 @@
       <c r="D169" s="17" t="s">
         <v>152</v>
       </c>
-      <c r="E169" s="17"/>
-      <c r="F169" s="17"/>
+      <c r="E169" s="17" t="s">
+        <v>201</v>
+      </c>
+      <c r="F169" s="17" t="s">
+        <v>183</v>
+      </c>
       <c r="G169" s="21">
         <v>22</v>
       </c>
@@ -6570,8 +7508,12 @@
       <c r="D170" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="E170" s="12"/>
-      <c r="F170" s="12"/>
+      <c r="E170" s="12" t="s">
+        <v>208</v>
+      </c>
+      <c r="F170" s="12" t="s">
+        <v>203</v>
+      </c>
       <c r="G170" s="13">
         <v>51</v>
       </c>
@@ -6602,8 +7544,12 @@
       <c r="D171" s="17" t="s">
         <v>151</v>
       </c>
-      <c r="E171" s="17"/>
-      <c r="F171" s="17"/>
+      <c r="E171" s="17" t="s">
+        <v>209</v>
+      </c>
+      <c r="F171" s="17" t="s">
+        <v>203</v>
+      </c>
       <c r="G171" s="21">
         <v>24</v>
       </c>
@@ -6634,8 +7580,12 @@
       <c r="D172" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="E172" s="12"/>
-      <c r="F172" s="12"/>
+      <c r="E172" s="12" t="s">
+        <v>211</v>
+      </c>
+      <c r="F172" s="12" t="s">
+        <v>203</v>
+      </c>
       <c r="G172" s="13">
         <v>2</v>
       </c>
@@ -6666,8 +7616,12 @@
       <c r="D173" s="17" t="s">
         <v>163</v>
       </c>
-      <c r="E173" s="17"/>
-      <c r="F173" s="17"/>
+      <c r="E173" s="17" t="s">
+        <v>255</v>
+      </c>
+      <c r="F173" s="17" t="s">
+        <v>183</v>
+      </c>
       <c r="G173" s="21">
         <v>38</v>
       </c>
@@ -6698,8 +7652,12 @@
       <c r="D174" s="12" t="s">
         <v>164</v>
       </c>
-      <c r="E174" s="12"/>
-      <c r="F174" s="12"/>
+      <c r="E174" s="12" t="s">
+        <v>256</v>
+      </c>
+      <c r="F174" s="12" t="s">
+        <v>183</v>
+      </c>
       <c r="G174" s="13">
         <v>10</v>
       </c>
@@ -6730,8 +7688,12 @@
       <c r="D175" s="17" t="s">
         <v>165</v>
       </c>
-      <c r="E175" s="17"/>
-      <c r="F175" s="17"/>
+      <c r="E175" s="17" t="s">
+        <v>219</v>
+      </c>
+      <c r="F175" s="17" t="s">
+        <v>185</v>
+      </c>
       <c r="G175" s="21">
         <v>8</v>
       </c>
@@ -6762,8 +7724,12 @@
       <c r="D176" s="12" t="s">
         <v>166</v>
       </c>
-      <c r="E176" s="12"/>
-      <c r="F176" s="12"/>
+      <c r="E176" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="F176" s="12" t="s">
+        <v>179</v>
+      </c>
       <c r="G176" s="13">
         <v>5</v>
       </c>
@@ -6794,8 +7760,12 @@
       <c r="D177" s="17" t="s">
         <v>127</v>
       </c>
-      <c r="E177" s="17"/>
-      <c r="F177" s="17"/>
+      <c r="E177" s="17" t="s">
+        <v>258</v>
+      </c>
+      <c r="F177" s="17" t="s">
+        <v>190</v>
+      </c>
       <c r="G177" s="21">
         <v>20</v>
       </c>
@@ -6826,8 +7796,12 @@
       <c r="D178" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="E178" s="12"/>
-      <c r="F178" s="12"/>
+      <c r="E178" s="12" t="s">
+        <v>202</v>
+      </c>
+      <c r="F178" s="12" t="s">
+        <v>203</v>
+      </c>
       <c r="G178" s="13">
         <v>26</v>
       </c>
@@ -6858,8 +7832,12 @@
       <c r="D179" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="E179" s="17"/>
-      <c r="F179" s="17"/>
+      <c r="E179" s="17" t="s">
+        <v>256</v>
+      </c>
+      <c r="F179" s="17" t="s">
+        <v>183</v>
+      </c>
       <c r="G179" s="21">
         <v>13</v>
       </c>
@@ -6890,8 +7868,12 @@
       <c r="D180" s="12" t="s">
         <v>130</v>
       </c>
-      <c r="E180" s="12"/>
-      <c r="F180" s="12"/>
+      <c r="E180" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="F180" s="12" t="s">
+        <v>179</v>
+      </c>
       <c r="G180" s="13">
         <v>8</v>
       </c>
@@ -6922,8 +7904,12 @@
       <c r="D181" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="E181" s="17"/>
-      <c r="F181" s="17"/>
+      <c r="E181" s="17" t="s">
+        <v>184</v>
+      </c>
+      <c r="F181" s="17" t="s">
+        <v>185</v>
+      </c>
       <c r="G181" s="21">
         <v>8</v>
       </c>
@@ -6954,8 +7940,12 @@
       <c r="D182" s="12" t="s">
         <v>142</v>
       </c>
-      <c r="E182" s="12"/>
-      <c r="F182" s="12"/>
+      <c r="E182" s="12" t="s">
+        <v>234</v>
+      </c>
+      <c r="F182" s="12" t="s">
+        <v>183</v>
+      </c>
       <c r="G182" s="13">
         <v>1</v>
       </c>
@@ -6986,8 +7976,12 @@
       <c r="D183" s="17" t="s">
         <v>166</v>
       </c>
-      <c r="E183" s="17"/>
-      <c r="F183" s="17"/>
+      <c r="E183" s="17" t="s">
+        <v>222</v>
+      </c>
+      <c r="F183" s="17" t="s">
+        <v>179</v>
+      </c>
       <c r="G183" s="21">
         <v>5</v>
       </c>
@@ -7018,8 +8012,12 @@
       <c r="D184" s="12" t="s">
         <v>164</v>
       </c>
-      <c r="E184" s="12"/>
-      <c r="F184" s="12"/>
+      <c r="E184" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="F184" s="12" t="s">
+        <v>179</v>
+      </c>
       <c r="G184" s="13">
         <v>10</v>
       </c>
@@ -7050,8 +8048,12 @@
       <c r="D185" s="17" t="s">
         <v>163</v>
       </c>
-      <c r="E185" s="17"/>
-      <c r="F185" s="17"/>
+      <c r="E185" s="17" t="s">
+        <v>257</v>
+      </c>
+      <c r="F185" s="17" t="s">
+        <v>179</v>
+      </c>
       <c r="G185" s="21">
         <v>38</v>
       </c>
@@ -7082,8 +8084,12 @@
       <c r="D186" s="12" t="s">
         <v>164</v>
       </c>
-      <c r="E186" s="12"/>
-      <c r="F186" s="12"/>
+      <c r="E186" s="12" t="s">
+        <v>258</v>
+      </c>
+      <c r="F186" s="12" t="s">
+        <v>190</v>
+      </c>
       <c r="G186" s="13">
         <v>10</v>
       </c>
@@ -7114,8 +8120,12 @@
       <c r="D187" s="17" t="s">
         <v>163</v>
       </c>
-      <c r="E187" s="17"/>
-      <c r="F187" s="17"/>
+      <c r="E187" s="17" t="s">
+        <v>258</v>
+      </c>
+      <c r="F187" s="17" t="s">
+        <v>190</v>
+      </c>
       <c r="G187" s="21">
         <v>38</v>
       </c>
@@ -7146,8 +8156,12 @@
       <c r="D188" s="12" t="s">
         <v>149</v>
       </c>
-      <c r="E188" s="12"/>
-      <c r="F188" s="12"/>
+      <c r="E188" s="12" t="s">
+        <v>244</v>
+      </c>
+      <c r="F188" s="12" t="s">
+        <v>190</v>
+      </c>
       <c r="G188" s="13">
         <v>31</v>
       </c>
@@ -7178,8 +8192,12 @@
       <c r="D189" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="E189" s="17"/>
-      <c r="F189" s="17"/>
+      <c r="E189" s="17" t="s">
+        <v>259</v>
+      </c>
+      <c r="F189" s="17" t="s">
+        <v>185</v>
+      </c>
       <c r="G189" s="21">
         <v>13</v>
       </c>
@@ -7210,8 +8228,12 @@
       <c r="D190" s="12" t="s">
         <v>158</v>
       </c>
-      <c r="E190" s="12"/>
-      <c r="F190" s="12"/>
+      <c r="E190" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="F190" s="12" t="s">
+        <v>185</v>
+      </c>
       <c r="G190" s="13">
         <v>9</v>
       </c>
@@ -7242,8 +8264,12 @@
       <c r="D191" s="17" t="s">
         <v>153</v>
       </c>
-      <c r="E191" s="17"/>
-      <c r="F191" s="17"/>
+      <c r="E191" s="17" t="s">
+        <v>260</v>
+      </c>
+      <c r="F191" s="17" t="s">
+        <v>190</v>
+      </c>
       <c r="G191" s="21">
         <v>47</v>
       </c>
@@ -7274,8 +8300,12 @@
       <c r="D192" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="E192" s="12"/>
-      <c r="F192" s="12"/>
+      <c r="E192" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="F192" s="12" t="s">
+        <v>179</v>
+      </c>
       <c r="G192" s="13">
         <v>20</v>
       </c>
@@ -7306,8 +8336,12 @@
       <c r="D193" s="17" t="s">
         <v>157</v>
       </c>
-      <c r="E193" s="17"/>
-      <c r="F193" s="17"/>
+      <c r="E193" s="17" t="s">
+        <v>261</v>
+      </c>
+      <c r="F193" s="17" t="s">
+        <v>197</v>
+      </c>
       <c r="G193" s="21">
         <v>111</v>
       </c>
@@ -7338,8 +8372,12 @@
       <c r="D194" s="12" t="s">
         <v>156</v>
       </c>
-      <c r="E194" s="12"/>
-      <c r="F194" s="12"/>
+      <c r="E194" s="12" t="s">
+        <v>262</v>
+      </c>
+      <c r="F194" s="12" t="s">
+        <v>185</v>
+      </c>
       <c r="G194" s="13">
         <v>117</v>
       </c>
@@ -7370,8 +8408,12 @@
       <c r="D195" s="17" t="s">
         <v>168</v>
       </c>
-      <c r="E195" s="17"/>
-      <c r="F195" s="17"/>
+      <c r="E195" s="17" t="s">
+        <v>263</v>
+      </c>
+      <c r="F195" s="17" t="s">
+        <v>185</v>
+      </c>
       <c r="G195" s="21">
         <v>35</v>
       </c>
@@ -7402,8 +8444,12 @@
       <c r="D196" s="12" t="s">
         <v>143</v>
       </c>
-      <c r="E196" s="12"/>
-      <c r="F196" s="12"/>
+      <c r="E196" s="12" t="s">
+        <v>235</v>
+      </c>
+      <c r="F196" s="12" t="s">
+        <v>181</v>
+      </c>
       <c r="G196" s="13">
         <v>30</v>
       </c>
@@ -7434,8 +8480,12 @@
       <c r="D197" s="17" t="s">
         <v>169</v>
       </c>
-      <c r="E197" s="17"/>
-      <c r="F197" s="17"/>
+      <c r="E197" s="17" t="s">
+        <v>249</v>
+      </c>
+      <c r="F197" s="17" t="s">
+        <v>190</v>
+      </c>
       <c r="G197" s="21">
         <v>45</v>
       </c>
@@ -7466,8 +8516,12 @@
       <c r="D198" s="12" t="s">
         <v>170</v>
       </c>
-      <c r="E198" s="12"/>
-      <c r="F198" s="12"/>
+      <c r="E198" s="12" t="s">
+        <v>251</v>
+      </c>
+      <c r="F198" s="12" t="s">
+        <v>190</v>
+      </c>
       <c r="G198" s="13">
         <v>10</v>
       </c>
@@ -7498,8 +8552,12 @@
       <c r="D199" s="17" t="s">
         <v>171</v>
       </c>
-      <c r="E199" s="17"/>
-      <c r="F199" s="17"/>
+      <c r="E199" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="F199" s="17" t="s">
+        <v>179</v>
+      </c>
       <c r="G199" s="21">
         <v>40</v>
       </c>
@@ -7530,8 +8588,12 @@
       <c r="D200" s="12" t="s">
         <v>172</v>
       </c>
-      <c r="E200" s="12"/>
-      <c r="F200" s="12"/>
+      <c r="E200" s="12" t="s">
+        <v>264</v>
+      </c>
+      <c r="F200" s="12" t="s">
+        <v>183</v>
+      </c>
       <c r="G200" s="13">
         <v>26</v>
       </c>
@@ -7562,8 +8624,12 @@
       <c r="D201" s="17" t="s">
         <v>173</v>
       </c>
-      <c r="E201" s="17"/>
-      <c r="F201" s="17"/>
+      <c r="E201" s="17" t="s">
+        <v>212</v>
+      </c>
+      <c r="F201" s="17" t="s">
+        <v>185</v>
+      </c>
       <c r="G201" s="21">
         <v>13</v>
       </c>
@@ -7590,7 +8656,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4294ACE-EA42-2E4B-9553-EFF45E9C82CE}">
   <dimension ref="A1:E304"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
@@ -7604,7 +8670,7 @@
       <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="29" t="s">
         <v>174</v>
       </c>
       <c r="C1" s="29" t="s">
@@ -7621,7 +8687,7 @@
       <c r="C2" s="31">
         <v>-3.2000000000000002E-3</v>
       </c>
-      <c r="E2" s="37"/>
+      <c r="E2" s="36"/>
     </row>
     <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="32">

</xml_diff>